<commit_message>
add groups to details report, #791
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/detail_report_template.xlsx
+++ b/bio_diversity/static/report_templates/detail_report_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Collection</t>
   </si>
@@ -1004,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I2"/>
+  <dimension ref="A2:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,32 +1021,35 @@
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>